<commit_message>
car_table and all FKs loaded
</commit_message>
<xml_diff>
--- a/sql-project-eo/sql-data-model.xlsx
+++ b/sql-project-eo/sql-data-model.xlsx
@@ -8,10 +8,10 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ericolsson/Library/Mobile Documents/com~apple~CloudDocs/👨🏻‍💻KeepCoding/Lesson Files/L15-18 SQL/sql-project-repo/sql-project-eo/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33621916-AD80-734F-8003-D3CFB4C3A047}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F234429E-72DD-CA41-9DF1-DC7855C39E89}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="23720" windowHeight="18880" xr2:uid="{57367D1F-08BC-D04B-80DE-952ACD0124DA}"/>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" activeTab="1" xr2:uid="{1278AF20-DA0E-D845-9634-9431A143D690}"/>
+    <workbookView xWindow="11600" yWindow="29560" windowWidth="23720" windowHeight="18880" activeTab="2" xr2:uid="{57367D1F-08BC-D04B-80DE-952ACD0124DA}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="51200" windowHeight="28300" activeTab="1" xr2:uid="{1278AF20-DA0E-D845-9634-9431A143D690}"/>
   </bookViews>
   <sheets>
     <sheet name="data_model" sheetId="1" r:id="rId1"/>
@@ -63,7 +63,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="489" uniqueCount="228">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="498" uniqueCount="230">
   <si>
     <t>Honda</t>
   </si>
@@ -747,6 +747,12 @@
   </si>
   <si>
     <t>FK to service_table</t>
+  </si>
+  <si>
+    <t>total_km</t>
+  </si>
+  <si>
+    <t>make last service amt?</t>
   </si>
 </sst>
 </file>
@@ -1252,8 +1258,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A25108A8-FD73-E34C-9782-50DCFCB93E9F}">
   <dimension ref="A1:M92"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A54" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12:B21"/>
+    <sheetView topLeftCell="A19" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="I11" sqref="I11"/>
     </sheetView>
     <sheetView workbookViewId="1">
       <selection sqref="A1:D1"/>
@@ -1279,21 +1285,21 @@
     <col min="17" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="35">
+    <row r="1" spans="1:9" ht="35">
       <c r="A1" s="14">
         <f ca="1">NOW()</f>
-        <v>44957.996531712961</v>
+        <v>44958.960784143521</v>
       </c>
       <c r="B1" s="14"/>
       <c r="C1" s="14"/>
       <c r="D1" s="14"/>
     </row>
-    <row r="3" spans="1:8">
+    <row r="3" spans="1:9">
       <c r="A3" s="1" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="10" spans="1:8" s="7" customFormat="1">
+    <row r="10" spans="1:9" s="7" customFormat="1">
       <c r="A10" s="8" t="s">
         <v>6</v>
       </c>
@@ -1316,8 +1322,11 @@
       <c r="H10" s="1" t="s">
         <v>112</v>
       </c>
-    </row>
-    <row r="11" spans="1:8">
+      <c r="I10" s="7" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9">
       <c r="A11" s="5" t="s">
         <v>89</v>
       </c>
@@ -1342,8 +1351,11 @@
       <c r="H11" s="6" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="12" spans="1:8">
+      <c r="I11" s="6" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9">
       <c r="A12" s="4">
         <v>1</v>
       </c>
@@ -1351,7 +1363,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="13" spans="1:8">
+    <row r="13" spans="1:9">
       <c r="A13" s="4">
         <v>2</v>
       </c>
@@ -1359,7 +1371,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="14" spans="1:8">
+    <row r="14" spans="1:9">
       <c r="A14" s="4">
         <v>3</v>
       </c>
@@ -1367,7 +1379,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="15" spans="1:8">
+    <row r="15" spans="1:9">
       <c r="A15" s="4">
         <v>4</v>
       </c>
@@ -1375,7 +1387,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="16" spans="1:8">
+    <row r="16" spans="1:9">
       <c r="A16" s="4">
         <v>5</v>
       </c>
@@ -2366,15 +2378,13 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BEF6DDA2-8713-044D-B08C-7FAD064AA1E7}">
-  <dimension ref="B1:I147"/>
+  <dimension ref="A1:I149"/>
   <sheetViews>
     <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
       <selection activeCell="D8" sqref="D8"/>
     </sheetView>
-    <sheetView tabSelected="1" topLeftCell="A92" zoomScale="110" zoomScaleNormal="110" workbookViewId="1">
-      <pane ySplit="10200" topLeftCell="A122" activePane="bottomLeft"/>
-      <selection activeCell="C107" sqref="C107:C116"/>
-      <selection pane="bottomLeft" activeCell="H126" sqref="H126:H135"/>
+    <sheetView tabSelected="1" topLeftCell="A95" zoomScale="110" zoomScaleNormal="110" workbookViewId="1">
+      <selection activeCell="I128" sqref="I128:I137"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" outlineLevelRow="1"/>
@@ -2385,7 +2395,7 @@
     <col min="6" max="6" width="19.33203125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="23.83203125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="16.6640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="118.5" customWidth="1"/>
+    <col min="9" max="9" width="144.5" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="6:9">
@@ -3077,7 +3087,7 @@
       <c r="E65" s="1"/>
       <c r="F65" s="1"/>
       <c r="G65" s="1"/>
-      <c r="H65" s="21" t="s">
+      <c r="H65" s="20" t="s">
         <v>219</v>
       </c>
       <c r="I65" s="22" t="str">
@@ -3356,7 +3366,7 @@
         <f>_xlfn.CONCAT("
 alter table kc_car_fleet_dll.",C65," 
 add constraint ",D66,"_FK foreign key (",D66,") 
-references kc_car_fleet_dll.",B124,"(",D66,")"
+references kc_car_fleet_dll.",A126,"(",D66,")"
 )</f>
         <v xml:space="preserve">
 alter table kc_car_fleet_dll.registration_table 
@@ -3365,7 +3375,7 @@
       </c>
     </row>
     <row r="81" spans="4:9">
-      <c r="H81" s="21" t="s">
+      <c r="H81" s="20" t="s">
         <v>219</v>
       </c>
       <c r="I81" t="str">
@@ -3389,7 +3399,7 @@
 G86," date not null, ",
 H86," date not null, 
 constraint ",D86,"_pk primary key(",D86,"));")</f>
-        <v>create table kc_car_fleet_dll.insurance_policy_table (ins_pol_id varchar(10) not null, car_id varchar(100)  not null, ins_co varchar(100)  not null, dt_ins_start date not null, dt_ins_end date not null, 
+        <v>create table kc_car_fleet_dll.insurance_policy_table (ins_pol_id varchar(10) not null, car_id varchar(100)  not null, ins_co_id varchar(100)  not null, dt_ins_start date not null, dt_ins_end date not null, 
 constraint ins_pol_id_pk primary key(ins_pol_id));</v>
       </c>
     </row>
@@ -3409,7 +3419,7 @@
       <c r="H85" s="7"/>
       <c r="I85" s="22" t="str">
         <f>CONCATENATE("insert into kc_car_fleet_dll.",D85," (",D86,", ",E86,", ",F86,", ",G86,", ",H86,") ")</f>
-        <v xml:space="preserve">insert into kc_car_fleet_dll.insurance_policy_table (ins_pol_id, car_id, ins_co, dt_ins_start, dt_ins_end) </v>
+        <v xml:space="preserve">insert into kc_car_fleet_dll.insurance_policy_table (ins_pol_id, car_id, ins_co_id, dt_ins_start, dt_ins_end) </v>
       </c>
     </row>
     <row r="86" spans="4:9">
@@ -3420,7 +3430,7 @@
         <v>89</v>
       </c>
       <c r="F86" s="6" t="s">
-        <v>136</v>
+        <v>97</v>
       </c>
       <c r="G86" s="6" t="s">
         <v>28</v>
@@ -3450,7 +3460,7 @@
       </c>
       <c r="I87" t="str">
         <f>CONCATENATE($I$85,"values('",D87,"','",E87,"','",F87,"','",G87,"','",H87,"');")</f>
-        <v>insert into kc_car_fleet_dll.insurance_policy_table (ins_pol_id, car_id, ins_co, dt_ins_start, dt_ins_end) values('P83723','2','3','2022-08-02','2023-08-01');</v>
+        <v>insert into kc_car_fleet_dll.insurance_policy_table (ins_pol_id, car_id, ins_co_id, dt_ins_start, dt_ins_end) values('P83723','2','3','2022-08-02','2023-08-01');</v>
       </c>
     </row>
     <row r="88" spans="4:9" ht="15" outlineLevel="1">
@@ -3471,7 +3481,7 @@
       </c>
       <c r="I88" t="str">
         <f t="shared" ref="I88:I96" si="6">CONCATENATE($I$85,"values('",D88,"','",E88,"','",F88,"','",G88,"','",H88,"');")</f>
-        <v>insert into kc_car_fleet_dll.insurance_policy_table (ins_pol_id, car_id, ins_co, dt_ins_start, dt_ins_end) values('P32508','10','2','2022-01-19','2023-01-18');</v>
+        <v>insert into kc_car_fleet_dll.insurance_policy_table (ins_pol_id, car_id, ins_co_id, dt_ins_start, dt_ins_end) values('P32508','10','2','2022-01-19','2023-01-18');</v>
       </c>
     </row>
     <row r="89" spans="4:9" ht="15" outlineLevel="1">
@@ -3492,7 +3502,7 @@
       </c>
       <c r="I89" t="str">
         <f t="shared" si="6"/>
-        <v>insert into kc_car_fleet_dll.insurance_policy_table (ins_pol_id, car_id, ins_co, dt_ins_start, dt_ins_end) values('P25409','8','3','2022-11-13','2023-11-12');</v>
+        <v>insert into kc_car_fleet_dll.insurance_policy_table (ins_pol_id, car_id, ins_co_id, dt_ins_start, dt_ins_end) values('P25409','8','3','2022-11-13','2023-11-12');</v>
       </c>
     </row>
     <row r="90" spans="4:9" ht="15" outlineLevel="1">
@@ -3513,7 +3523,7 @@
       </c>
       <c r="I90" t="str">
         <f t="shared" si="6"/>
-        <v>insert into kc_car_fleet_dll.insurance_policy_table (ins_pol_id, car_id, ins_co, dt_ins_start, dt_ins_end) values('P71722','9','1','2022-01-14','2023-01-13');</v>
+        <v>insert into kc_car_fleet_dll.insurance_policy_table (ins_pol_id, car_id, ins_co_id, dt_ins_start, dt_ins_end) values('P71722','9','1','2022-01-14','2023-01-13');</v>
       </c>
     </row>
     <row r="91" spans="4:9" ht="15" outlineLevel="1">
@@ -3534,7 +3544,7 @@
       </c>
       <c r="I91" t="str">
         <f t="shared" si="6"/>
-        <v>insert into kc_car_fleet_dll.insurance_policy_table (ins_pol_id, car_id, ins_co, dt_ins_start, dt_ins_end) values('P36494','7','2','2022-07-25','2023-07-24');</v>
+        <v>insert into kc_car_fleet_dll.insurance_policy_table (ins_pol_id, car_id, ins_co_id, dt_ins_start, dt_ins_end) values('P36494','7','2','2022-07-25','2023-07-24');</v>
       </c>
     </row>
     <row r="92" spans="4:9" ht="15" outlineLevel="1">
@@ -3555,7 +3565,7 @@
       </c>
       <c r="I92" t="str">
         <f t="shared" si="6"/>
-        <v>insert into kc_car_fleet_dll.insurance_policy_table (ins_pol_id, car_id, ins_co, dt_ins_start, dt_ins_end) values('P31162','1','2','2022-07-25','2023-07-24');</v>
+        <v>insert into kc_car_fleet_dll.insurance_policy_table (ins_pol_id, car_id, ins_co_id, dt_ins_start, dt_ins_end) values('P31162','1','2','2022-07-25','2023-07-24');</v>
       </c>
     </row>
     <row r="93" spans="4:9" ht="15" outlineLevel="1">
@@ -3576,7 +3586,7 @@
       </c>
       <c r="I93" t="str">
         <f t="shared" si="6"/>
-        <v>insert into kc_car_fleet_dll.insurance_policy_table (ins_pol_id, car_id, ins_co, dt_ins_start, dt_ins_end) values('P73660','3','2','2022-01-29','2023-01-28');</v>
+        <v>insert into kc_car_fleet_dll.insurance_policy_table (ins_pol_id, car_id, ins_co_id, dt_ins_start, dt_ins_end) values('P73660','3','2','2022-01-29','2023-01-28');</v>
       </c>
     </row>
     <row r="94" spans="4:9" ht="15" outlineLevel="1">
@@ -3597,7 +3607,7 @@
       </c>
       <c r="I94" t="str">
         <f t="shared" si="6"/>
-        <v>insert into kc_car_fleet_dll.insurance_policy_table (ins_pol_id, car_id, ins_co, dt_ins_start, dt_ins_end) values('P85940','4','2','2022-07-28','2023-07-27');</v>
+        <v>insert into kc_car_fleet_dll.insurance_policy_table (ins_pol_id, car_id, ins_co_id, dt_ins_start, dt_ins_end) values('P85940','4','2','2022-07-28','2023-07-27');</v>
       </c>
     </row>
     <row r="95" spans="4:9" ht="15" outlineLevel="1">
@@ -3618,7 +3628,7 @@
       </c>
       <c r="I95" t="str">
         <f t="shared" si="6"/>
-        <v>insert into kc_car_fleet_dll.insurance_policy_table (ins_pol_id, car_id, ins_co, dt_ins_start, dt_ins_end) values('P43571','6','3','2022-02-08','2023-02-07');</v>
+        <v>insert into kc_car_fleet_dll.insurance_policy_table (ins_pol_id, car_id, ins_co_id, dt_ins_start, dt_ins_end) values('P43571','6','3','2022-02-08','2023-02-07');</v>
       </c>
     </row>
     <row r="96" spans="4:9" ht="15" outlineLevel="1">
@@ -3639,7 +3649,7 @@
       </c>
       <c r="I96" t="str">
         <f t="shared" si="6"/>
-        <v>insert into kc_car_fleet_dll.insurance_policy_table (ins_pol_id, car_id, ins_co, dt_ins_start, dt_ins_end) values('P31802','5','2','2022-08-14','2023-08-13');</v>
+        <v>insert into kc_car_fleet_dll.insurance_policy_table (ins_pol_id, car_id, ins_co_id, dt_ins_start, dt_ins_end) values('P31802','5','2','2022-08-14','2023-08-13');</v>
       </c>
     </row>
     <row r="99" spans="3:9">
@@ -3650,7 +3660,7 @@
         <f>_xlfn.CONCAT("
 alter table kc_car_fleet_dll.",D85," 
 add constraint ",E86,"_FK foreign key (",E86,") 
-references kc_car_fleet_dll.",B124,"(",E86,")"
+references kc_car_fleet_dll.",A126,"(",E86,")"
 )</f>
         <v xml:space="preserve">
 alter table kc_car_fleet_dll.insurance_policy_table 
@@ -3659,7 +3669,7 @@
       </c>
     </row>
     <row r="100" spans="3:9">
-      <c r="H100" s="21" t="s">
+      <c r="H100" s="20" t="s">
         <v>220</v>
       </c>
       <c r="I100" t="str">
@@ -3670,8 +3680,8 @@
 )</f>
         <v xml:space="preserve">
 alter table kc_car_fleet_dll.insurance_policy_table 
-add constraint ins_co_FK foreign key (ins_co) 
-references kc_car_fleet_dll.insurance_company_table(ins_co)</v>
+add constraint ins_co_id_FK foreign key (ins_co_id) 
+references kc_car_fleet_dll.insurance_company_table(ins_co_id)</v>
       </c>
     </row>
     <row r="104" spans="3:9">
@@ -3747,11 +3757,11 @@
       </c>
       <c r="H107" s="1">
         <f ca="1">RANDBETWEEN(1,3)</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="I107" t="str">
         <f ca="1">CONCATENATE($I$105,"values('",C107,"','",D107,"','",E107,"','",F107,"','",G107,"','",H107,"');")</f>
-        <v>insert into kc_car_fleet_dll.service_table (service_id, car_id, odometer_km, dt_service, service_amount, curr_id) values('S009','1','38229','2022-08-30','564','2');</v>
+        <v>insert into kc_car_fleet_dll.service_table (service_id, car_id, odometer_km, dt_service, service_amount, curr_id) values('S009','1','38229','2022-08-30','564','3');</v>
       </c>
     </row>
     <row r="108" spans="3:9" outlineLevel="1">
@@ -3874,7 +3884,7 @@
         <v>insert into kc_car_fleet_dll.service_table (service_id, car_id, odometer_km, dt_service, service_amount, curr_id) values('S006','6','46120','2022-10-15','590','2');</v>
       </c>
     </row>
-    <row r="113" spans="2:9" outlineLevel="1">
+    <row r="113" spans="1:9" outlineLevel="1">
       <c r="C113" s="1" t="s">
         <v>204</v>
       </c>
@@ -3898,7 +3908,7 @@
         <v>insert into kc_car_fleet_dll.service_table (service_id, car_id, odometer_km, dt_service, service_amount, curr_id) values('S004','7','61918','2022-09-22','343','1');</v>
       </c>
     </row>
-    <row r="114" spans="2:9" outlineLevel="1">
+    <row r="114" spans="1:9" outlineLevel="1">
       <c r="C114" s="1" t="s">
         <v>205</v>
       </c>
@@ -3922,7 +3932,7 @@
         <v>insert into kc_car_fleet_dll.service_table (service_id, car_id, odometer_km, dt_service, service_amount, curr_id) values('S005','8','41353','2022-10-13','296','1');</v>
       </c>
     </row>
-    <row r="115" spans="2:9" outlineLevel="1">
+    <row r="115" spans="1:9" outlineLevel="1">
       <c r="C115" s="1" t="s">
         <v>206</v>
       </c>
@@ -3946,7 +3956,7 @@
         <v>insert into kc_car_fleet_dll.service_table (service_id, car_id, odometer_km, dt_service, service_amount, curr_id) values('S003','9','28804','2022-05-26','499','2');</v>
       </c>
     </row>
-    <row r="116" spans="2:9" outlineLevel="1">
+    <row r="116" spans="1:9" outlineLevel="1">
       <c r="C116" s="1" t="s">
         <v>207</v>
       </c>
@@ -3970,12 +3980,12 @@
         <v>insert into kc_car_fleet_dll.service_table (service_id, car_id, odometer_km, dt_service, service_amount, curr_id) values('S001','10','36878','2022-11-29','201','1');</v>
       </c>
     </row>
-    <row r="119" spans="2:9">
+    <row r="119" spans="1:9">
       <c r="I119" t="s">
         <v>217</v>
       </c>
     </row>
-    <row r="120" spans="2:9">
+    <row r="120" spans="1:9">
       <c r="H120" s="21" t="s">
         <v>218</v>
       </c>
@@ -3983,7 +3993,7 @@
         <f>_xlfn.CONCAT("
 alter table kc_car_fleet_dll.",C105," 
 add constraint ",D106,"_FK foreign key (",D106,") 
-references kc_car_fleet_dll.",B124,"(",D106,")"
+references kc_car_fleet_dll.",A126,"(",D106,")"
 )</f>
         <v xml:space="preserve">
 alter table kc_car_fleet_dll.service_table 
@@ -3991,8 +4001,8 @@
 references kc_car_fleet_dll.car_table(car_id)</v>
       </c>
     </row>
-    <row r="121" spans="2:9">
-      <c r="H121" s="21" t="s">
+    <row r="121" spans="1:9">
+      <c r="H121" s="20" t="s">
         <v>219</v>
       </c>
       <c r="I121" t="str">
@@ -4007,320 +4017,438 @@
 references kc_car_fleet_dll.currency_table(curr_id)</v>
       </c>
     </row>
-    <row r="124" spans="2:9">
-      <c r="B124" s="8" t="s">
+    <row r="125" spans="1:9">
+      <c r="I125" t="str">
+        <f>CONCATENATE("create table kc_car_fleet_dll.",A126," (",
+A127," varchar(10) not null, ",
+B127," date not null, ",
+C127," varchar(10) not null, ",
+D127," varchar(10) not null, ",
+E127," varchar(100) not null, ",
+F127," varchar(100) not null, ",
+G127," varchar(10) not null, ",
+H127," varchar(10) not null, constraint ",A127,"_pk primary key(",A127,"));")</f>
+        <v>create table kc_car_fleet_dll.car_table (car_id varchar(10) not null, dt_purchased date not null, model_id varchar(10) not null, color_id varchar(10) not null, license_plate_id varchar(100) not null, ins_pol_id varchar(100) not null, service_id varchar(10) not null, total_km varchar(10) not null, constraint car_id_pk primary key(car_id));</v>
+      </c>
+    </row>
+    <row r="126" spans="1:9">
+      <c r="A126" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="C124" s="8"/>
-      <c r="D124" s="21" t="s">
+      <c r="B126" s="8"/>
+      <c r="C126" s="21" t="s">
         <v>223</v>
       </c>
-      <c r="E124" s="21" t="s">
+      <c r="D126" s="21" t="s">
         <v>224</v>
       </c>
-      <c r="F124" s="21" t="s">
+      <c r="E126" s="21" t="s">
         <v>225</v>
       </c>
-      <c r="G124" s="21" t="s">
+      <c r="F126" s="21" t="s">
         <v>226</v>
       </c>
-      <c r="H124" s="21" t="s">
+      <c r="G126" s="21" t="s">
         <v>227</v>
       </c>
-    </row>
-    <row r="125" spans="2:9">
-      <c r="B125" s="5" t="s">
+      <c r="I126" s="22" t="str">
+        <f>CONCATENATE("insert into kc_car_fleet_dll.",A126," (",A127,", ",B127,", ",C127,", ",D127,", ",E127,", ",F127,", ",G127,", ",H127,") ")</f>
+        <v xml:space="preserve">insert into kc_car_fleet_dll.car_table (car_id, dt_purchased, model_id, color_id, license_plate_id, ins_pol_id, service_id, total_km) </v>
+      </c>
+    </row>
+    <row r="127" spans="1:9">
+      <c r="A127" s="5" t="s">
         <v>89</v>
       </c>
-      <c r="C125" s="6" t="s">
+      <c r="B127" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="D125" s="6" t="s">
+      <c r="C127" s="6" t="s">
         <v>95</v>
       </c>
-      <c r="E125" s="6" t="s">
+      <c r="D127" s="6" t="s">
         <v>96</v>
       </c>
-      <c r="F125" s="6" t="s">
+      <c r="E127" s="6" t="s">
         <v>134</v>
       </c>
-      <c r="G125" s="19" t="s">
+      <c r="F127" s="19" t="s">
         <v>93</v>
       </c>
-      <c r="H125" s="6" t="s">
+      <c r="G127" s="6" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="126" spans="2:9" ht="15">
-      <c r="B126" s="1">
-        <v>1</v>
-      </c>
-      <c r="C126" s="17" t="s">
+      <c r="H127" s="6" t="s">
+        <v>228</v>
+      </c>
+      <c r="I127" s="10" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="128" spans="1:9" ht="15">
+      <c r="A128" s="1">
+        <v>1</v>
+      </c>
+      <c r="B128" s="17" t="s">
         <v>187</v>
       </c>
-      <c r="D126" s="1">
+      <c r="C128" s="1">
         <f ca="1">RANDBETWEEN(1,14)</f>
-        <v>13</v>
-      </c>
-      <c r="E126" s="1">
+        <v>10</v>
+      </c>
+      <c r="D128" s="1">
         <f ca="1">RANDBETWEEN(1,4)</f>
         <v>4</v>
       </c>
-      <c r="F126" s="1" t="s">
+      <c r="E128" s="1" t="s">
         <v>122</v>
       </c>
-      <c r="G126" s="16" t="s">
+      <c r="F128" s="16" t="s">
         <v>142</v>
       </c>
-      <c r="H126" s="1" t="s">
+      <c r="G128" s="1" t="s">
         <v>198</v>
       </c>
-    </row>
-    <row r="127" spans="2:9" ht="15">
-      <c r="B127" s="1">
-        <v>2</v>
-      </c>
-      <c r="C127" s="17" t="s">
+      <c r="H128" s="1">
+        <v>49657</v>
+      </c>
+      <c r="I128" t="str">
+        <f ca="1">CONCATENATE($I$126,"values('",A128,"','",B128,"','",C128,"','",D128,"','",E128,"','",F128,"','",G128,"','",H128,"');")</f>
+        <v>insert into kc_car_fleet_dll.car_table (car_id, dt_purchased, model_id, color_id, license_plate_id, ins_pol_id, service_id, total_km) values('1','2018-10-26','10','4','BGM937','P31162','S009','49657');</v>
+      </c>
+    </row>
+    <row r="129" spans="1:9" ht="15">
+      <c r="A129" s="1">
+        <v>2</v>
+      </c>
+      <c r="B129" s="17" t="s">
         <v>188</v>
       </c>
-      <c r="D127" s="1">
-        <f t="shared" ref="D127:D135" ca="1" si="8">RANDBETWEEN(1,14)</f>
+      <c r="C129" s="1">
+        <f t="shared" ref="C129:C137" ca="1" si="8">RANDBETWEEN(1,14)</f>
+        <v>7</v>
+      </c>
+      <c r="D129" s="1">
+        <f t="shared" ref="D129:D137" ca="1" si="9">RANDBETWEEN(1,4)</f>
+        <v>2</v>
+      </c>
+      <c r="E129" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="F129" s="16" t="s">
+        <v>137</v>
+      </c>
+      <c r="G129" s="1" t="s">
+        <v>199</v>
+      </c>
+      <c r="H129" s="1">
+        <v>64896</v>
+      </c>
+      <c r="I129" t="str">
+        <f t="shared" ref="I129:I137" ca="1" si="10">CONCATENATE($I$126,"values('",A129,"','",B129,"','",C129,"','",D129,"','",E129,"','",F129,"','",G129,"','",H129,"');")</f>
+        <v>insert into kc_car_fleet_dll.car_table (car_id, dt_purchased, model_id, color_id, license_plate_id, ins_pol_id, service_id, total_km) values('2','2018-05-29','7','2','TYC246','P83723','S007','64896');</v>
+      </c>
+    </row>
+    <row r="130" spans="1:9" ht="15">
+      <c r="A130" s="1">
+        <v>3</v>
+      </c>
+      <c r="B130" s="17" t="s">
+        <v>189</v>
+      </c>
+      <c r="C130" s="1">
+        <f t="shared" ca="1" si="8"/>
+        <v>5</v>
+      </c>
+      <c r="D130" s="1">
+        <f t="shared" ca="1" si="9"/>
+        <v>4</v>
+      </c>
+      <c r="E130" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="F130" s="16" t="s">
+        <v>143</v>
+      </c>
+      <c r="G130" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="H130" s="1">
+        <v>52524</v>
+      </c>
+      <c r="I130" t="str">
+        <f t="shared" ca="1" si="10"/>
+        <v>insert into kc_car_fleet_dll.car_table (car_id, dt_purchased, model_id, color_id, license_plate_id, ins_pol_id, service_id, total_km) values('3','2018-09-10','5','4','VXK5925','P73660','S008','52524');</v>
+      </c>
+    </row>
+    <row r="131" spans="1:9" ht="15">
+      <c r="A131" s="1">
+        <v>4</v>
+      </c>
+      <c r="B131" s="17" t="s">
+        <v>190</v>
+      </c>
+      <c r="C131" s="1">
+        <f t="shared" ca="1" si="8"/>
+        <v>6</v>
+      </c>
+      <c r="D131" s="1">
+        <f t="shared" ca="1" si="9"/>
+        <v>2</v>
+      </c>
+      <c r="E131" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="F131" s="16" t="s">
+        <v>144</v>
+      </c>
+      <c r="G131" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="H131" s="1">
+        <v>77935</v>
+      </c>
+      <c r="I131" t="str">
+        <f t="shared" ca="1" si="10"/>
+        <v>insert into kc_car_fleet_dll.car_table (car_id, dt_purchased, model_id, color_id, license_plate_id, ins_pol_id, service_id, total_km) values('4','2018-03-13','6','2','UQO8298','P85940','S010','77935');</v>
+      </c>
+    </row>
+    <row r="132" spans="1:9" ht="15">
+      <c r="A132" s="1">
+        <v>5</v>
+      </c>
+      <c r="B132" s="17" t="s">
+        <v>191</v>
+      </c>
+      <c r="C132" s="1">
+        <f t="shared" ca="1" si="8"/>
+        <v>7</v>
+      </c>
+      <c r="D132" s="1">
+        <f t="shared" ca="1" si="9"/>
+        <v>1</v>
+      </c>
+      <c r="E132" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="F132" s="16" t="s">
+        <v>146</v>
+      </c>
+      <c r="G132" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="H132" s="1">
+        <v>49589</v>
+      </c>
+      <c r="I132" t="str">
+        <f t="shared" ca="1" si="10"/>
+        <v>insert into kc_car_fleet_dll.car_table (car_id, dt_purchased, model_id, color_id, license_plate_id, ins_pol_id, service_id, total_km) values('5','2016-03-22','7','1','ELO2020','P31802','S002','49589');</v>
+      </c>
+    </row>
+    <row r="133" spans="1:9" ht="15">
+      <c r="A133" s="1">
+        <v>6</v>
+      </c>
+      <c r="B133" s="17" t="s">
+        <v>135</v>
+      </c>
+      <c r="C133" s="1">
+        <f t="shared" ca="1" si="8"/>
+        <v>2</v>
+      </c>
+      <c r="D133" s="1">
+        <f t="shared" ca="1" si="9"/>
+        <v>3</v>
+      </c>
+      <c r="E133" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="F133" s="16" t="s">
+        <v>145</v>
+      </c>
+      <c r="G133" s="1" t="s">
+        <v>203</v>
+      </c>
+      <c r="H133" s="1">
+        <v>66840</v>
+      </c>
+      <c r="I133" t="str">
+        <f t="shared" ca="1" si="10"/>
+        <v>insert into kc_car_fleet_dll.car_table (car_id, dt_purchased, model_id, color_id, license_plate_id, ins_pol_id, service_id, total_km) values('6','2018-06-23','2','3','ZTW2748','P43571','S006','66840');</v>
+      </c>
+    </row>
+    <row r="134" spans="1:9" ht="15">
+      <c r="A134" s="1">
+        <v>7</v>
+      </c>
+      <c r="B134" s="17" t="s">
+        <v>192</v>
+      </c>
+      <c r="C134" s="1">
+        <f t="shared" ca="1" si="8"/>
+        <v>2</v>
+      </c>
+      <c r="D134" s="1">
+        <f t="shared" ca="1" si="9"/>
+        <v>1</v>
+      </c>
+      <c r="E134" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="F134" s="16" t="s">
+        <v>141</v>
+      </c>
+      <c r="G134" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="H134" s="1">
+        <v>79469</v>
+      </c>
+      <c r="I134" t="str">
+        <f t="shared" ca="1" si="10"/>
+        <v>insert into kc_car_fleet_dll.car_table (car_id, dt_purchased, model_id, color_id, license_plate_id, ins_pol_id, service_id, total_km) values('7','2020-02-02','2','1','RSP6195','P36494','S004','79469');</v>
+      </c>
+    </row>
+    <row r="135" spans="1:9" ht="15">
+      <c r="A135" s="1">
         <v>8</v>
       </c>
-      <c r="E127" s="1">
-        <f t="shared" ref="E127:E135" ca="1" si="9">RANDBETWEEN(1,4)</f>
-        <v>4</v>
-      </c>
-      <c r="F127" s="1" t="s">
-        <v>123</v>
-      </c>
-      <c r="G127" s="16" t="s">
-        <v>137</v>
-      </c>
-      <c r="H127" s="1" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="128" spans="2:9" ht="15">
-      <c r="B128" s="1">
-        <v>3</v>
-      </c>
-      <c r="C128" s="17" t="s">
-        <v>189</v>
-      </c>
-      <c r="D128" s="1">
+      <c r="B135" s="17" t="s">
+        <v>193</v>
+      </c>
+      <c r="C135" s="1">
         <f t="shared" ca="1" si="8"/>
         <v>8</v>
       </c>
-      <c r="E128" s="1">
+      <c r="D135" s="1">
         <f t="shared" ca="1" si="9"/>
-        <v>3</v>
-      </c>
-      <c r="F128" s="1" t="s">
-        <v>124</v>
-      </c>
-      <c r="G128" s="16" t="s">
-        <v>143</v>
-      </c>
-      <c r="H128" s="1" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="129" spans="2:8" ht="15">
-      <c r="B129" s="1">
-        <v>4</v>
-      </c>
-      <c r="C129" s="17" t="s">
-        <v>190</v>
-      </c>
-      <c r="D129" s="1">
+        <v>2</v>
+      </c>
+      <c r="E135" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="F135" s="16" t="s">
+        <v>139</v>
+      </c>
+      <c r="G135" s="1" t="s">
+        <v>205</v>
+      </c>
+      <c r="H135" s="1">
+        <v>42893</v>
+      </c>
+      <c r="I135" t="str">
+        <f t="shared" ca="1" si="10"/>
+        <v>insert into kc_car_fleet_dll.car_table (car_id, dt_purchased, model_id, color_id, license_plate_id, ins_pol_id, service_id, total_km) values('8','2016-11-10','8','2','LUH4314','P25409','S005','42893');</v>
+      </c>
+    </row>
+    <row r="136" spans="1:9" ht="15">
+      <c r="A136" s="1">
+        <v>9</v>
+      </c>
+      <c r="B136" s="17" t="s">
+        <v>194</v>
+      </c>
+      <c r="C136" s="1">
         <f t="shared" ca="1" si="8"/>
-        <v>2</v>
-      </c>
-      <c r="E129" s="1">
+        <v>7</v>
+      </c>
+      <c r="D136" s="1">
         <f t="shared" ca="1" si="9"/>
-        <v>2</v>
-      </c>
-      <c r="F129" s="1" t="s">
-        <v>125</v>
-      </c>
-      <c r="G129" s="16" t="s">
-        <v>144</v>
-      </c>
-      <c r="H129" s="1" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="130" spans="2:8" ht="15">
-      <c r="B130" s="1">
-        <v>5</v>
-      </c>
-      <c r="C130" s="17" t="s">
-        <v>191</v>
-      </c>
-      <c r="D130" s="1">
+        <v>1</v>
+      </c>
+      <c r="E136" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="F136" s="16" t="s">
+        <v>140</v>
+      </c>
+      <c r="G136" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="H136" s="1">
+        <v>31526</v>
+      </c>
+      <c r="I136" t="str">
+        <f t="shared" ca="1" si="10"/>
+        <v>insert into kc_car_fleet_dll.car_table (car_id, dt_purchased, model_id, color_id, license_plate_id, ins_pol_id, service_id, total_km) values('9','2019-08-09','7','1','HZI6923','P71722','S003','31526');</v>
+      </c>
+    </row>
+    <row r="137" spans="1:9" ht="15">
+      <c r="A137" s="1">
+        <v>10</v>
+      </c>
+      <c r="B137" s="17" t="s">
+        <v>195</v>
+      </c>
+      <c r="C137" s="1">
         <f t="shared" ca="1" si="8"/>
-        <v>1</v>
-      </c>
-      <c r="E130" s="1">
+        <v>9</v>
+      </c>
+      <c r="D137" s="1">
         <f t="shared" ca="1" si="9"/>
-        <v>3</v>
-      </c>
-      <c r="F130" s="1" t="s">
-        <v>126</v>
-      </c>
-      <c r="G130" s="16" t="s">
-        <v>146</v>
-      </c>
-      <c r="H130" s="1" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="131" spans="2:8" ht="15">
-      <c r="B131" s="1">
-        <v>6</v>
-      </c>
-      <c r="C131" s="17" t="s">
-        <v>135</v>
-      </c>
-      <c r="D131" s="1">
-        <f t="shared" ca="1" si="8"/>
-        <v>4</v>
-      </c>
-      <c r="E131" s="1">
-        <f t="shared" ca="1" si="9"/>
-        <v>3</v>
-      </c>
-      <c r="F131" s="1" t="s">
-        <v>127</v>
-      </c>
-      <c r="G131" s="16" t="s">
-        <v>145</v>
-      </c>
-      <c r="H131" s="1" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="132" spans="2:8" ht="15">
-      <c r="B132" s="1">
-        <v>7</v>
-      </c>
-      <c r="C132" s="17" t="s">
-        <v>192</v>
-      </c>
-      <c r="D132" s="1">
-        <f t="shared" ca="1" si="8"/>
-        <v>12</v>
-      </c>
-      <c r="E132" s="1">
-        <f t="shared" ca="1" si="9"/>
-        <v>3</v>
-      </c>
-      <c r="F132" s="1" t="s">
-        <v>128</v>
-      </c>
-      <c r="G132" s="16" t="s">
-        <v>141</v>
-      </c>
-      <c r="H132" s="1" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="133" spans="2:8" ht="15">
-      <c r="B133" s="1">
-        <v>8</v>
-      </c>
-      <c r="C133" s="17" t="s">
-        <v>193</v>
-      </c>
-      <c r="D133" s="1">
-        <f t="shared" ca="1" si="8"/>
-        <v>6</v>
-      </c>
-      <c r="E133" s="1">
-        <f t="shared" ca="1" si="9"/>
-        <v>4</v>
-      </c>
-      <c r="F133" s="1" t="s">
-        <v>129</v>
-      </c>
-      <c r="G133" s="16" t="s">
-        <v>139</v>
-      </c>
-      <c r="H133" s="1" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="134" spans="2:8" ht="15">
-      <c r="B134" s="1">
-        <v>9</v>
-      </c>
-      <c r="C134" s="17" t="s">
-        <v>194</v>
-      </c>
-      <c r="D134" s="1">
-        <f t="shared" ca="1" si="8"/>
-        <v>1</v>
-      </c>
-      <c r="E134" s="1">
-        <f t="shared" ca="1" si="9"/>
-        <v>4</v>
-      </c>
-      <c r="F134" s="1" t="s">
-        <v>130</v>
-      </c>
-      <c r="G134" s="16" t="s">
-        <v>140</v>
-      </c>
-      <c r="H134" s="1" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="135" spans="2:8" ht="15">
-      <c r="B135" s="1">
-        <v>10</v>
-      </c>
-      <c r="C135" s="17" t="s">
-        <v>195</v>
-      </c>
-      <c r="D135" s="1">
-        <f t="shared" ca="1" si="8"/>
-        <v>8</v>
-      </c>
-      <c r="E135" s="1">
-        <f t="shared" ca="1" si="9"/>
-        <v>4</v>
-      </c>
-      <c r="F135" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E137" s="1" t="s">
         <v>131</v>
       </c>
-      <c r="G135" s="16" t="s">
+      <c r="F137" s="16" t="s">
         <v>138</v>
       </c>
-      <c r="H135" s="1" t="s">
+      <c r="G137" s="1" t="s">
         <v>207</v>
       </c>
-    </row>
-    <row r="138" spans="2:8">
-      <c r="H138" s="1"/>
-    </row>
-    <row r="139" spans="2:8">
-      <c r="H139" s="1"/>
-    </row>
-    <row r="140" spans="2:8">
-      <c r="H140" s="1"/>
-    </row>
-    <row r="141" spans="2:8">
-      <c r="H141" s="1"/>
-    </row>
-    <row r="142" spans="2:8">
-      <c r="H142" s="1"/>
-    </row>
-    <row r="143" spans="2:8">
-      <c r="H143" s="1"/>
-    </row>
-    <row r="144" spans="2:8">
-      <c r="H144" s="1"/>
+      <c r="H137" s="1">
+        <v>37321</v>
+      </c>
+      <c r="I137" t="str">
+        <f t="shared" ca="1" si="10"/>
+        <v>insert into kc_car_fleet_dll.car_table (car_id, dt_purchased, model_id, color_id, license_plate_id, ins_pol_id, service_id, total_km) values('10','2016-02-26','9','2','ZLO5123','P32508','S001','37321');</v>
+      </c>
+    </row>
+    <row r="140" spans="1:9">
+      <c r="H140" s="21" t="s">
+        <v>223</v>
+      </c>
+      <c r="I140" t="str">
+        <f>_xlfn.CONCAT("alter table kc_car_fleet_dll.",A126," add constraint ",C127,"_FK foreign key (",C127,") references kc_car_fleet_dll.",F21,"(",C127,");")</f>
+        <v>alter table kc_car_fleet_dll.car_table add constraint model_id_FK foreign key (model_id) references kc_car_fleet_dll.model_table(model_id);</v>
+      </c>
+    </row>
+    <row r="141" spans="1:9">
+      <c r="H141" s="21" t="s">
+        <v>224</v>
+      </c>
+      <c r="I141" t="str">
+        <f>_xlfn.CONCAT("alter table kc_car_fleet_dll.",A126," add constraint ",D127,"_FK foreign key (",D127,") references kc_car_fleet_dll.",G39,"(",D127,");")</f>
+        <v>alter table kc_car_fleet_dll.car_table add constraint color_id_FK foreign key (color_id) references kc_car_fleet_dll.color_table(color_id);</v>
+      </c>
+    </row>
+    <row r="142" spans="1:9">
+      <c r="H142" s="21" t="s">
+        <v>225</v>
+      </c>
+      <c r="I142" t="str">
+        <f>_xlfn.CONCAT("alter table kc_car_fleet_dll.",A126," add constraint ",E127,"_FK foreign key (",E127,") references kc_car_fleet_dll.",C65,"(",E127,");")</f>
+        <v>alter table kc_car_fleet_dll.car_table add constraint license_plate_id_FK foreign key (license_plate_id) references kc_car_fleet_dll.registration_table(license_plate_id);</v>
+      </c>
+    </row>
+    <row r="143" spans="1:9">
+      <c r="H143" s="21" t="s">
+        <v>226</v>
+      </c>
+      <c r="I143" t="str">
+        <f>_xlfn.CONCAT("alter table kc_car_fleet_dll.",A126," add constraint ",F127,"_FK foreign key (",F127,") references kc_car_fleet_dll.",D85,"(",F127,");")</f>
+        <v>alter table kc_car_fleet_dll.car_table add constraint ins_pol_id_FK foreign key (ins_pol_id) references kc_car_fleet_dll.insurance_policy_table(ins_pol_id);</v>
+      </c>
+    </row>
+    <row r="144" spans="1:9">
+      <c r="H144" s="21" t="s">
+        <v>227</v>
+      </c>
+      <c r="I144" t="str">
+        <f>_xlfn.CONCAT("alter table kc_car_fleet_dll.",A126," add constraint ",G127,"_FK foreign key (",G127,") references kc_car_fleet_dll.",C105,"(",G127,");")</f>
+        <v>alter table kc_car_fleet_dll.car_table add constraint service_id_FK foreign key (service_id) references kc_car_fleet_dll.service_table(service_id);</v>
+      </c>
     </row>
     <row r="145" spans="8:8">
       <c r="H145" s="1"/>
@@ -4331,9 +4459,15 @@
     <row r="147" spans="8:8">
       <c r="H147" s="1"/>
     </row>
+    <row r="148" spans="8:8">
+      <c r="H148" s="1"/>
+    </row>
+    <row r="149" spans="8:8">
+      <c r="H149" s="1"/>
+    </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="G138:H147">
-    <sortCondition ref="H138:H147"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="G140:H149">
+    <sortCondition ref="H140:H149"/>
   </sortState>
   <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4345,7 +4479,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{304935D2-0CBF-5044-B3DC-3854351AD42F}">
   <dimension ref="A1:J43"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
     <sheetView workbookViewId="1">
@@ -4446,30 +4580,30 @@
       </c>
       <c r="B5" s="16" t="str">
         <f ca="1">CHAR(RANDBETWEEN(65,90))&amp;CHAR(RANDBETWEEN(65,90))&amp;CHAR(RANDBETWEEN(65,90))&amp;RANDBETWEEN(0,99)&amp;RANDBETWEEN(10,99)</f>
-        <v>WEA1635</v>
+        <v>NDA8724</v>
       </c>
       <c r="C5" s="15">
         <v>44479</v>
       </c>
       <c r="D5" s="1">
         <f ca="1">RANDBETWEEN(D$2,D$1)</f>
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="E5" s="1">
         <f t="shared" ref="E5:F14" ca="1" si="0">RANDBETWEEN(E$2,E$1)</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F5" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="I5" s="15">
         <f t="shared" ref="I5:I14" ca="1" si="1">RANDBETWEEN(I$2,I$1)</f>
-        <v>44682</v>
+        <v>44890</v>
       </c>
       <c r="J5" s="11">
         <f ca="1">I5+364</f>
-        <v>45046</v>
+        <v>45254</v>
       </c>
     </row>
     <row r="6" spans="1:10" ht="15">
@@ -4478,14 +4612,14 @@
       </c>
       <c r="B6" s="16" t="str">
         <f ca="1">CHAR(RANDBETWEEN(65,90))&amp;CHAR(RANDBETWEEN(65,90))&amp;CHAR(RANDBETWEEN(65,90))&amp;RANDBETWEEN(0,99)&amp;RANDBETWEEN(10,99)</f>
-        <v>ORU7817</v>
+        <v>IWQ6759</v>
       </c>
       <c r="C6" s="15">
         <v>44329</v>
       </c>
       <c r="D6" s="1">
         <f ca="1">RANDBETWEEN(D$2,D$1)</f>
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="E6" s="1">
         <f t="shared" ca="1" si="0"/>
@@ -4497,11 +4631,11 @@
       </c>
       <c r="I6" s="15">
         <f t="shared" ca="1" si="1"/>
-        <v>44677</v>
+        <v>44901</v>
       </c>
       <c r="J6" s="11">
         <f t="shared" ref="J6:J14" ca="1" si="2">I6+364</f>
-        <v>45041</v>
+        <v>45265</v>
       </c>
     </row>
     <row r="7" spans="1:10" ht="15">
@@ -4510,14 +4644,14 @@
       </c>
       <c r="B7" s="16" t="str">
         <f ca="1">CHAR(RANDBETWEEN(65,90))&amp;CHAR(RANDBETWEEN(65,90))&amp;CHAR(RANDBETWEEN(65,90))&amp;RANDBETWEEN(0,99)&amp;RANDBETWEEN(10,99)</f>
-        <v>BIB6155</v>
+        <v>RRN761</v>
       </c>
       <c r="C7" s="15">
         <v>44433</v>
       </c>
       <c r="D7" s="1">
         <f ca="1">RANDBETWEEN(D$2,D$1)</f>
-        <v>4</v>
+        <v>13</v>
       </c>
       <c r="E7" s="1">
         <f t="shared" ca="1" si="0"/>
@@ -4525,15 +4659,15 @@
       </c>
       <c r="F7" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="I7" s="15">
         <f t="shared" ca="1" si="1"/>
-        <v>44581</v>
+        <v>44629</v>
       </c>
       <c r="J7" s="11">
         <f t="shared" ca="1" si="2"/>
-        <v>44945</v>
+        <v>44993</v>
       </c>
     </row>
     <row r="8" spans="1:10" ht="15">
@@ -4542,18 +4676,18 @@
       </c>
       <c r="B8" s="16" t="str">
         <f ca="1">CHAR(RANDBETWEEN(65,90))&amp;CHAR(RANDBETWEEN(65,90))&amp;CHAR(RANDBETWEEN(65,90))&amp;RANDBETWEEN(0,99)&amp;RANDBETWEEN(10,99)</f>
-        <v>GZG3636</v>
+        <v>UUZ8623</v>
       </c>
       <c r="C8" s="15">
         <v>44252</v>
       </c>
       <c r="D8" s="1">
         <f ca="1">RANDBETWEEN(D$2,D$1)</f>
-        <v>13</v>
+        <v>3</v>
       </c>
       <c r="E8" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F8" s="1">
         <f t="shared" ca="1" si="0"/>
@@ -4561,11 +4695,11 @@
       </c>
       <c r="I8" s="15">
         <f t="shared" ca="1" si="1"/>
-        <v>44766</v>
+        <v>44673</v>
       </c>
       <c r="J8" s="11">
         <f t="shared" ca="1" si="2"/>
-        <v>45130</v>
+        <v>45037</v>
       </c>
     </row>
     <row r="9" spans="1:10" ht="15">
@@ -4574,7 +4708,7 @@
       </c>
       <c r="B9" s="16" t="str">
         <f ca="1">CHAR(RANDBETWEEN(65,90))&amp;CHAR(RANDBETWEEN(65,90))&amp;CHAR(RANDBETWEEN(65,90))&amp;RANDBETWEEN(0,99)&amp;RANDBETWEEN(10,99)</f>
-        <v>POP9272</v>
+        <v>NOG5436</v>
       </c>
       <c r="C9" s="15">
         <v>43531</v>
@@ -4585,19 +4719,19 @@
       </c>
       <c r="E9" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F9" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="I9" s="15">
         <f t="shared" ca="1" si="1"/>
-        <v>44738</v>
+        <v>44744</v>
       </c>
       <c r="J9" s="11">
         <f t="shared" ca="1" si="2"/>
-        <v>45102</v>
+        <v>45108</v>
       </c>
     </row>
     <row r="10" spans="1:10" ht="15">
@@ -4606,30 +4740,30 @@
       </c>
       <c r="B10" s="16" t="str">
         <f ca="1">CHAR(RANDBETWEEN(65,90))&amp;CHAR(RANDBETWEEN(65,90))&amp;CHAR(RANDBETWEEN(65,90))&amp;RANDBETWEEN(0,99)&amp;RANDBETWEEN(10,99)</f>
-        <v>OJI7876</v>
+        <v>MKA9437</v>
       </c>
       <c r="C10" s="15">
         <v>43984</v>
       </c>
       <c r="D10" s="1">
         <f ca="1">RANDBETWEEN(D$2,D$1)</f>
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="E10" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F10" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="I10" s="15">
         <f t="shared" ca="1" si="1"/>
-        <v>44839</v>
+        <v>44716</v>
       </c>
       <c r="J10" s="11">
         <f t="shared" ca="1" si="2"/>
-        <v>45203</v>
+        <v>45080</v>
       </c>
     </row>
     <row r="11" spans="1:10" ht="15">
@@ -4638,30 +4772,30 @@
       </c>
       <c r="B11" s="16" t="str">
         <f ca="1">CHAR(RANDBETWEEN(65,90))&amp;CHAR(RANDBETWEEN(65,90))&amp;CHAR(RANDBETWEEN(65,90))&amp;RANDBETWEEN(0,99)&amp;RANDBETWEEN(10,99)</f>
-        <v>YKV5897</v>
+        <v>UOU7818</v>
       </c>
       <c r="C11" s="15">
         <v>44943</v>
       </c>
       <c r="D11" s="1">
         <f ca="1">RANDBETWEEN(D$2,D$1)</f>
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="E11" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F11" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="I11" s="15">
         <f t="shared" ca="1" si="1"/>
-        <v>44906</v>
+        <v>44923</v>
       </c>
       <c r="J11" s="11">
         <f t="shared" ca="1" si="2"/>
-        <v>45270</v>
+        <v>45287</v>
       </c>
     </row>
     <row r="12" spans="1:10" ht="15">
@@ -4670,30 +4804,30 @@
       </c>
       <c r="B12" s="16" t="str">
         <f ca="1">CHAR(RANDBETWEEN(65,90))&amp;CHAR(RANDBETWEEN(65,90))&amp;CHAR(RANDBETWEEN(65,90))&amp;RANDBETWEEN(0,99)&amp;RANDBETWEEN(10,99)</f>
-        <v>YVI1331</v>
+        <v>FWC9465</v>
       </c>
       <c r="C12" s="15">
         <v>43394</v>
       </c>
       <c r="D12" s="1">
         <f ca="1">RANDBETWEEN(D$2,D$1)</f>
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="E12" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F12" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="I12" s="15">
         <f t="shared" ca="1" si="1"/>
-        <v>44701</v>
+        <v>44670</v>
       </c>
       <c r="J12" s="11">
         <f t="shared" ca="1" si="2"/>
-        <v>45065</v>
+        <v>45034</v>
       </c>
     </row>
     <row r="13" spans="1:10" ht="15">
@@ -4702,18 +4836,18 @@
       </c>
       <c r="B13" s="16" t="str">
         <f ca="1">CHAR(RANDBETWEEN(65,90))&amp;CHAR(RANDBETWEEN(65,90))&amp;CHAR(RANDBETWEEN(65,90))&amp;RANDBETWEEN(0,99)&amp;RANDBETWEEN(10,99)</f>
-        <v>WLL138</v>
+        <v>PUC3635</v>
       </c>
       <c r="C13" s="15">
         <v>44396</v>
       </c>
       <c r="D13" s="1">
         <f ca="1">RANDBETWEEN(D$2,D$1)</f>
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="E13" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F13" s="1">
         <f t="shared" ca="1" si="0"/>
@@ -4721,11 +4855,11 @@
       </c>
       <c r="I13" s="15">
         <f t="shared" ca="1" si="1"/>
-        <v>44864</v>
+        <v>44732</v>
       </c>
       <c r="J13" s="11">
         <f t="shared" ca="1" si="2"/>
-        <v>45228</v>
+        <v>45096</v>
       </c>
     </row>
     <row r="14" spans="1:10" ht="15">
@@ -4734,7 +4868,7 @@
       </c>
       <c r="B14" s="16" t="str">
         <f ca="1">CHAR(RANDBETWEEN(65,90))&amp;CHAR(RANDBETWEEN(65,90))&amp;CHAR(RANDBETWEEN(65,90))&amp;RANDBETWEEN(0,99)&amp;RANDBETWEEN(10,99)</f>
-        <v>JMD3359</v>
+        <v>DNT2695</v>
       </c>
       <c r="C14" s="15">
         <v>43136</v>
@@ -4745,19 +4879,19 @@
       </c>
       <c r="E14" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="F14" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="I14" s="15">
         <f t="shared" ca="1" si="1"/>
-        <v>44653</v>
+        <v>44677</v>
       </c>
       <c r="J14" s="11">
         <f t="shared" ca="1" si="2"/>
-        <v>45017</v>
+        <v>45041</v>
       </c>
     </row>
     <row r="18" spans="2:10">
@@ -4793,7 +4927,7 @@
     <row r="21" spans="2:10" ht="15">
       <c r="B21" s="16" t="str">
         <f t="shared" ref="B21:B30" ca="1" si="3">"P"&amp;RANDBETWEEN(10000,99999)</f>
-        <v>P42096</v>
+        <v>P86290</v>
       </c>
       <c r="I21" s="17" t="s">
         <v>173</v>
@@ -4805,7 +4939,7 @@
     <row r="22" spans="2:10" ht="15">
       <c r="B22" s="16" t="str">
         <f ca="1">"P"&amp;RANDBETWEEN(10000,99999)</f>
-        <v>P85957</v>
+        <v>P77788</v>
       </c>
       <c r="I22" s="17" t="s">
         <v>175</v>
@@ -4817,7 +4951,7 @@
     <row r="23" spans="2:10" ht="15">
       <c r="B23" s="16" t="str">
         <f t="shared" ref="B23:B30" ca="1" si="4">"P"&amp;RANDBETWEEN(10000,99999)</f>
-        <v>P22338</v>
+        <v>P22528</v>
       </c>
       <c r="I23" s="17" t="s">
         <v>177</v>
@@ -4829,7 +4963,7 @@
     <row r="24" spans="2:10" ht="15">
       <c r="B24" s="16" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>P35390</v>
+        <v>P92574</v>
       </c>
       <c r="I24" s="17" t="s">
         <v>179</v>
@@ -4841,7 +4975,7 @@
     <row r="25" spans="2:10" ht="15">
       <c r="B25" s="16" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>P57288</v>
+        <v>P59245</v>
       </c>
       <c r="I25" s="17" t="s">
         <v>181</v>
@@ -4853,7 +4987,7 @@
     <row r="26" spans="2:10" ht="15">
       <c r="B26" s="16" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>P38660</v>
+        <v>P57254</v>
       </c>
       <c r="I26" s="17" t="s">
         <v>183</v>
@@ -4865,7 +4999,7 @@
     <row r="27" spans="2:10" ht="15">
       <c r="B27" s="16" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>P10352</v>
+        <v>P25286</v>
       </c>
       <c r="I27" s="17" t="s">
         <v>185</v>
@@ -4877,19 +5011,19 @@
     <row r="28" spans="2:10" ht="15">
       <c r="B28" s="16" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>P13923</v>
+        <v>P45675</v>
       </c>
     </row>
     <row r="29" spans="2:10" ht="15">
       <c r="B29" s="16" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>P77052</v>
+        <v>P93329</v>
       </c>
     </row>
     <row r="30" spans="2:10" ht="15">
       <c r="B30" s="16" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>P58755</v>
+        <v>P96035</v>
       </c>
     </row>
     <row r="33" spans="4:5">
@@ -4906,7 +5040,7 @@
       </c>
       <c r="E34" s="1" cm="1">
         <f t="array" aca="1" ref="E34:E43" ca="1">_xlfn.SORTBY(D34:D43,_xlfn.RANDARRAY(COUNTA(D34:D43)))</f>
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="35" spans="4:5">
@@ -4915,7 +5049,7 @@
       </c>
       <c r="E35" s="1">
         <f ca="1"/>
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="36" spans="4:5">
@@ -4924,7 +5058,7 @@
       </c>
       <c r="E36" s="1">
         <f ca="1"/>
-        <v>4</v>
+        <v>10</v>
       </c>
     </row>
     <row r="37" spans="4:5">
@@ -4933,7 +5067,7 @@
       </c>
       <c r="E37" s="1">
         <f ca="1"/>
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="38" spans="4:5">
@@ -4942,7 +5076,7 @@
       </c>
       <c r="E38" s="1">
         <f ca="1"/>
-        <v>3</v>
+        <v>9</v>
       </c>
     </row>
     <row r="39" spans="4:5">
@@ -4951,7 +5085,7 @@
       </c>
       <c r="E39" s="1">
         <f ca="1"/>
-        <v>1</v>
+        <v>7</v>
       </c>
     </row>
     <row r="40" spans="4:5">
@@ -4960,7 +5094,7 @@
       </c>
       <c r="E40" s="1">
         <f ca="1"/>
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="41" spans="4:5">
@@ -4969,7 +5103,7 @@
       </c>
       <c r="E41" s="1">
         <f ca="1"/>
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="42" spans="4:5">
@@ -4978,7 +5112,7 @@
       </c>
       <c r="E42" s="1">
         <f ca="1"/>
-        <v>6</v>
+        <v>2</v>
       </c>
     </row>
     <row r="43" spans="4:5">
@@ -4987,7 +5121,7 @@
       </c>
       <c r="E43" s="1">
         <f ca="1"/>
-        <v>7</v>
+        <v>3</v>
       </c>
     </row>
   </sheetData>
@@ -5383,331 +5517,331 @@
     <row r="5" spans="1:3">
       <c r="B5" s="11">
         <f ca="1">RANDBETWEEN($B$1,$B$2)</f>
-        <v>44367</v>
+        <v>44082</v>
       </c>
       <c r="C5" s="11">
         <f ca="1">B5+364</f>
-        <v>44731</v>
+        <v>44446</v>
       </c>
     </row>
     <row r="6" spans="1:3">
       <c r="B6" s="11">
         <f t="shared" ref="B6:B37" ca="1" si="0">RANDBETWEEN($B$1,$B$2)</f>
-        <v>43965</v>
+        <v>43406</v>
       </c>
       <c r="C6" s="11">
         <f t="shared" ref="C6:C37" ca="1" si="1">B6+364</f>
-        <v>44329</v>
+        <v>43770</v>
       </c>
     </row>
     <row r="7" spans="1:3">
       <c r="B7" s="11">
         <f t="shared" ca="1" si="0"/>
-        <v>43595</v>
+        <v>43470</v>
       </c>
       <c r="C7" s="11">
         <f t="shared" ca="1" si="1"/>
-        <v>43959</v>
+        <v>43834</v>
       </c>
     </row>
     <row r="8" spans="1:3">
       <c r="B8" s="11">
         <f t="shared" ca="1" si="0"/>
-        <v>43675</v>
+        <v>44333</v>
       </c>
       <c r="C8" s="11">
         <f t="shared" ca="1" si="1"/>
-        <v>44039</v>
+        <v>44697</v>
       </c>
     </row>
     <row r="9" spans="1:3">
       <c r="B9" s="11">
         <f t="shared" ca="1" si="0"/>
-        <v>43905</v>
+        <v>44827</v>
       </c>
       <c r="C9" s="11">
         <f t="shared" ca="1" si="1"/>
-        <v>44269</v>
+        <v>45191</v>
       </c>
     </row>
     <row r="10" spans="1:3">
       <c r="B10" s="11">
         <f t="shared" ca="1" si="0"/>
-        <v>44691</v>
+        <v>43883</v>
       </c>
       <c r="C10" s="11">
         <f t="shared" ca="1" si="1"/>
-        <v>45055</v>
+        <v>44247</v>
       </c>
     </row>
     <row r="11" spans="1:3">
       <c r="B11" s="11">
         <f t="shared" ca="1" si="0"/>
-        <v>44843</v>
+        <v>44404</v>
       </c>
       <c r="C11" s="11">
         <f t="shared" ca="1" si="1"/>
-        <v>45207</v>
+        <v>44768</v>
       </c>
     </row>
     <row r="12" spans="1:3">
       <c r="B12" s="11">
         <f t="shared" ca="1" si="0"/>
-        <v>43666</v>
+        <v>43839</v>
       </c>
       <c r="C12" s="11">
         <f t="shared" ca="1" si="1"/>
-        <v>44030</v>
+        <v>44203</v>
       </c>
     </row>
     <row r="13" spans="1:3">
       <c r="B13" s="11">
         <f t="shared" ca="1" si="0"/>
-        <v>43314</v>
+        <v>43316</v>
       </c>
       <c r="C13" s="11">
         <f t="shared" ca="1" si="1"/>
-        <v>43678</v>
+        <v>43680</v>
       </c>
     </row>
     <row r="14" spans="1:3">
       <c r="B14" s="11">
         <f t="shared" ca="1" si="0"/>
-        <v>44726</v>
+        <v>43609</v>
       </c>
       <c r="C14" s="11">
         <f t="shared" ca="1" si="1"/>
-        <v>45090</v>
+        <v>43973</v>
       </c>
     </row>
     <row r="15" spans="1:3">
       <c r="B15" s="11">
         <f t="shared" ca="1" si="0"/>
-        <v>44430</v>
+        <v>43720</v>
       </c>
       <c r="C15" s="11">
         <f t="shared" ca="1" si="1"/>
-        <v>44794</v>
+        <v>44084</v>
       </c>
     </row>
     <row r="16" spans="1:3">
       <c r="B16" s="11">
         <f t="shared" ca="1" si="0"/>
-        <v>43410</v>
+        <v>43317</v>
       </c>
       <c r="C16" s="11">
         <f t="shared" ca="1" si="1"/>
-        <v>43774</v>
+        <v>43681</v>
       </c>
     </row>
     <row r="17" spans="2:3">
       <c r="B17" s="11">
         <f t="shared" ca="1" si="0"/>
-        <v>43755</v>
+        <v>44900</v>
       </c>
       <c r="C17" s="11">
         <f t="shared" ca="1" si="1"/>
-        <v>44119</v>
+        <v>45264</v>
       </c>
     </row>
     <row r="18" spans="2:3">
       <c r="B18" s="11">
         <f t="shared" ca="1" si="0"/>
-        <v>44830</v>
+        <v>44160</v>
       </c>
       <c r="C18" s="11">
         <f t="shared" ca="1" si="1"/>
-        <v>45194</v>
+        <v>44524</v>
       </c>
     </row>
     <row r="19" spans="2:3">
       <c r="B19" s="11">
         <f t="shared" ca="1" si="0"/>
-        <v>43157</v>
+        <v>44524</v>
       </c>
       <c r="C19" s="11">
         <f t="shared" ca="1" si="1"/>
-        <v>43521</v>
+        <v>44888</v>
       </c>
     </row>
     <row r="20" spans="2:3">
       <c r="B20" s="11">
         <f t="shared" ca="1" si="0"/>
-        <v>43967</v>
+        <v>44779</v>
       </c>
       <c r="C20" s="11">
         <f t="shared" ca="1" si="1"/>
-        <v>44331</v>
+        <v>45143</v>
       </c>
     </row>
     <row r="21" spans="2:3">
       <c r="B21" s="11">
         <f t="shared" ca="1" si="0"/>
-        <v>43609</v>
+        <v>44947</v>
       </c>
       <c r="C21" s="11">
         <f t="shared" ca="1" si="1"/>
-        <v>43973</v>
+        <v>45311</v>
       </c>
     </row>
     <row r="22" spans="2:3">
       <c r="B22" s="11">
         <f t="shared" ca="1" si="0"/>
-        <v>44627</v>
+        <v>44435</v>
       </c>
       <c r="C22" s="11">
         <f t="shared" ca="1" si="1"/>
-        <v>44991</v>
+        <v>44799</v>
       </c>
     </row>
     <row r="23" spans="2:3">
       <c r="B23" s="11">
         <f t="shared" ca="1" si="0"/>
-        <v>43887</v>
+        <v>43691</v>
       </c>
       <c r="C23" s="11">
         <f t="shared" ca="1" si="1"/>
-        <v>44251</v>
+        <v>44055</v>
       </c>
     </row>
     <row r="24" spans="2:3">
       <c r="B24" s="11">
         <f t="shared" ca="1" si="0"/>
-        <v>44138</v>
+        <v>44651</v>
       </c>
       <c r="C24" s="11">
         <f t="shared" ca="1" si="1"/>
-        <v>44502</v>
+        <v>45015</v>
       </c>
     </row>
     <row r="25" spans="2:3">
       <c r="B25" s="11">
         <f t="shared" ca="1" si="0"/>
-        <v>43714</v>
+        <v>44848</v>
       </c>
       <c r="C25" s="11">
         <f t="shared" ca="1" si="1"/>
-        <v>44078</v>
+        <v>45212</v>
       </c>
     </row>
     <row r="26" spans="2:3">
       <c r="B26" s="11">
         <f t="shared" ca="1" si="0"/>
-        <v>43855</v>
+        <v>43626</v>
       </c>
       <c r="C26" s="11">
         <f t="shared" ca="1" si="1"/>
-        <v>44219</v>
+        <v>43990</v>
       </c>
     </row>
     <row r="27" spans="2:3">
       <c r="B27" s="11">
         <f t="shared" ca="1" si="0"/>
-        <v>43529</v>
+        <v>44008</v>
       </c>
       <c r="C27" s="11">
         <f t="shared" ca="1" si="1"/>
-        <v>43893</v>
+        <v>44372</v>
       </c>
     </row>
     <row r="28" spans="2:3">
       <c r="B28" s="11">
         <f t="shared" ca="1" si="0"/>
-        <v>43525</v>
+        <v>43692</v>
       </c>
       <c r="C28" s="11">
         <f t="shared" ca="1" si="1"/>
-        <v>43889</v>
+        <v>44056</v>
       </c>
     </row>
     <row r="29" spans="2:3">
       <c r="B29" s="11">
         <f t="shared" ca="1" si="0"/>
-        <v>43818</v>
+        <v>44414</v>
       </c>
       <c r="C29" s="11">
         <f t="shared" ca="1" si="1"/>
-        <v>44182</v>
+        <v>44778</v>
       </c>
     </row>
     <row r="30" spans="2:3">
       <c r="B30" s="11">
         <f t="shared" ca="1" si="0"/>
-        <v>43802</v>
+        <v>43780</v>
       </c>
       <c r="C30" s="11">
         <f t="shared" ca="1" si="1"/>
-        <v>44166</v>
+        <v>44144</v>
       </c>
     </row>
     <row r="31" spans="2:3">
       <c r="B31" s="11">
         <f t="shared" ca="1" si="0"/>
-        <v>43783</v>
+        <v>43547</v>
       </c>
       <c r="C31" s="11">
         <f t="shared" ca="1" si="1"/>
-        <v>44147</v>
+        <v>43911</v>
       </c>
     </row>
     <row r="32" spans="2:3">
       <c r="B32" s="11">
         <f t="shared" ca="1" si="0"/>
-        <v>43691</v>
+        <v>44895</v>
       </c>
       <c r="C32" s="11">
         <f t="shared" ca="1" si="1"/>
-        <v>44055</v>
+        <v>45259</v>
       </c>
     </row>
     <row r="33" spans="2:3">
       <c r="B33" s="11">
         <f t="shared" ca="1" si="0"/>
-        <v>43125</v>
+        <v>43268</v>
       </c>
       <c r="C33" s="11">
         <f t="shared" ca="1" si="1"/>
-        <v>43489</v>
+        <v>43632</v>
       </c>
     </row>
     <row r="34" spans="2:3">
       <c r="B34" s="11">
         <f t="shared" ca="1" si="0"/>
-        <v>44733</v>
+        <v>43654</v>
       </c>
       <c r="C34" s="11">
         <f t="shared" ca="1" si="1"/>
-        <v>45097</v>
+        <v>44018</v>
       </c>
     </row>
     <row r="35" spans="2:3">
       <c r="B35" s="11">
         <f t="shared" ca="1" si="0"/>
-        <v>43392</v>
+        <v>43305</v>
       </c>
       <c r="C35" s="11">
         <f t="shared" ca="1" si="1"/>
-        <v>43756</v>
+        <v>43669</v>
       </c>
     </row>
     <row r="36" spans="2:3">
       <c r="B36" s="11">
         <f t="shared" ca="1" si="0"/>
-        <v>43726</v>
+        <v>43813</v>
       </c>
       <c r="C36" s="11">
         <f t="shared" ca="1" si="1"/>
-        <v>44090</v>
+        <v>44177</v>
       </c>
     </row>
     <row r="37" spans="2:3">
       <c r="B37" s="11">
         <f t="shared" ca="1" si="0"/>
-        <v>43888</v>
+        <v>44494</v>
       </c>
       <c r="C37" s="11">
         <f t="shared" ca="1" si="1"/>
-        <v>44252</v>
+        <v>44858</v>
       </c>
     </row>
   </sheetData>

</xml_diff>